<commit_message>
McCormick envelopes added to the ESSs' model.
</commit_message>
<xml_diff>
--- a/data/HR1_2/A_KPC_35_1/A_KPC_35_1_base.xlsx
+++ b/data/HR1_2/A_KPC_35_1/A_KPC_35_1_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\HR1_2\A_KPC_35_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3E7D08-23E3-4971-9877-2C75F07DD3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DB6F15-D70A-48B6-9E0B-1DEAD0FB38CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -69,6 +69,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,10 +549,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -908,7 +912,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,15 +933,15 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.2500000000000001E-2</v>
+      <c r="B2" s="3">
+        <v>5.0000000000000004E-6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -945,16 +949,16 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.5000000000000001E-2</v>
+      <c r="B4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.01</v>
+      <c r="B5" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC5C45B-EC79-4B34-93BA-F1E16EABD698}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -4813,7 +4817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023FB202-3806-4902-BB26-726E6591C8FF}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>